<commit_message>
penambahan lattitude dan longtittude
</commit_message>
<xml_diff>
--- a/Documents/DIAGRAM STUDI KASUS V.4.1.xlsx
+++ b/Documents/DIAGRAM STUDI KASUS V.4.1.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="224">
   <si>
     <t>Arrival : -</t>
   </si>
@@ -54,9 +54,6 @@
     <t>EVENT : PERTEMUAN PENGAWAS</t>
   </si>
   <si>
-    <t>Waktu Mulai : 19. 00 WIB</t>
-  </si>
-  <si>
     <t>Waktu Selesai : 21.30 WIB</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>RUMAH</t>
   </si>
   <si>
-    <t>Maleber, KarangTengah, Cianjur</t>
-  </si>
-  <si>
     <t>Motor(62.2Km, 132 menit)</t>
   </si>
   <si>
@@ -87,9 +81,6 @@
     <t>"font berwarna merah" transportasi yg dipilih</t>
   </si>
   <si>
-    <t xml:space="preserve"> Jl. Aceh No. 71 A, Citarum, Bandung Wetan</t>
-  </si>
-  <si>
     <t>Departure : -</t>
   </si>
   <si>
@@ -123,30 +114,15 @@
     <t>EVENT : ISTIRAHAT</t>
   </si>
   <si>
-    <t>Waktu Mulai : 22. 00 WIB</t>
-  </si>
-  <si>
     <t>Waktu Selesai : 06.00 WIB</t>
   </si>
   <si>
-    <t>Jalan Citarum No.23, Citarum, Bandung</t>
-  </si>
-  <si>
     <t>Mobil(0.75Km, 8menit)</t>
   </si>
   <si>
     <t>Jalan Kaki(1Km, 15 menit)</t>
   </si>
   <si>
-    <t>Bus()</t>
-  </si>
-  <si>
-    <t>Pesawat()</t>
-  </si>
-  <si>
-    <t>kereta api()</t>
-  </si>
-  <si>
     <t>Jalan Kaki(77.85Km, 740 menit)</t>
   </si>
   <si>
@@ -156,15 +132,9 @@
     <t>EVENT :  ISHOMA</t>
   </si>
   <si>
-    <t>Waktu Mulai : 13.15 WIB</t>
-  </si>
-  <si>
     <t>Waktu Selesai : 15.00 WIB</t>
   </si>
   <si>
-    <t>Jl. Citarum No.3A, Citarum, Bandung</t>
-  </si>
-  <si>
     <t>Jalan Kaki(0.17Km, 2 menit)</t>
   </si>
   <si>
@@ -180,9 +150,6 @@
     <t>Waktu Selesai : 18.00 WIB</t>
   </si>
   <si>
-    <t>Waktu Mulai : 18.10 WIB</t>
-  </si>
-  <si>
     <t>Waktu Selesai : 19.00 WIB</t>
   </si>
   <si>
@@ -264,9 +231,6 @@
     <t>EVENT [7]</t>
   </si>
   <si>
-    <t>Waktu Mulai : 08.00 WIB</t>
-  </si>
-  <si>
     <t>Jalan Kaki(10.3 Km, 127 menit)</t>
   </si>
   <si>
@@ -291,9 +255,6 @@
     <t>Departure : 15.25 WIB</t>
   </si>
   <si>
-    <t xml:space="preserve">Jl. Parang Kusumo No.2-I, Kemayoran,  Surabaya </t>
-  </si>
-  <si>
     <t>Jalan Kaki(13.6 Km, 170 menit)</t>
   </si>
   <si>
@@ -318,9 +279,6 @@
     <t>EVENT [8]</t>
   </si>
   <si>
-    <t>Jl. Rajawali No.9-11 Krembangan, Surabaya</t>
-  </si>
-  <si>
     <t>EVENT :  CHECK IN HOTEL</t>
   </si>
   <si>
@@ -348,9 +306,6 @@
     <t>Waktu Selesai : 07.45 WIB</t>
   </si>
   <si>
-    <t>Jl. Dukuh Menanggal Sel. No.103 Kota SBY,</t>
-  </si>
-  <si>
     <t>EVENT [8.1]</t>
   </si>
   <si>
@@ -361,9 +316,6 @@
   </si>
   <si>
     <t>DINAS PENDIDIKAN KAB CIANJUR,</t>
-  </si>
-  <si>
-    <t>Jl. Perintis Kemerdekaan No. 3, Cilaku, Kabupaten Cianjur</t>
   </si>
   <si>
     <t>EVENT [11]</t>
@@ -584,12 +536,6 @@
     <t>Mobil'umum'(10.3 Km,22 menit)</t>
   </si>
   <si>
-    <t>(08.00 - 0.10) - 0.22 = 7.28(MOBIL)</t>
-  </si>
-  <si>
-    <t>(08.00 - 0.10) - 2.07 = 05.43(JALAN KAKI)</t>
-  </si>
-  <si>
     <t>Motor(10.3 Km, 20 menit)</t>
   </si>
   <si>
@@ -650,12 +596,6 @@
     <t>Departure : 04.54 WIB</t>
   </si>
   <si>
-    <t>(08.00 - 0.10) - 0.20 = 7.30(MOTOR)</t>
-  </si>
-  <si>
-    <t>Departure : 07.28 WIB</t>
-  </si>
-  <si>
     <t>Arrival : 06.50 WIB</t>
   </si>
   <si>
@@ -671,12 +611,6 @@
     <t>Arrival : 05.10 WIB</t>
   </si>
   <si>
-    <t>Arrival : 07.50 WIB</t>
-  </si>
-  <si>
-    <t>Waktu Selesai : 07.25 WIB</t>
-  </si>
-  <si>
     <t>Departure : 19.18 WIB</t>
   </si>
   <si>
@@ -701,15 +635,6 @@
     <t>Pesawat : LION AIR  JT 911 (Boeing 737-800)</t>
   </si>
   <si>
-    <t>Bus(unknown)</t>
-  </si>
-  <si>
-    <t>Pesawat(unknown)</t>
-  </si>
-  <si>
-    <t>kereta api(unknown)</t>
-  </si>
-  <si>
     <t>tanggal : 22 Oktober 2017 pukul: 20.10 - 21.00</t>
   </si>
   <si>
@@ -717,6 +642,81 @@
   </si>
   <si>
     <t>Bus(tidak rute)</t>
+  </si>
+  <si>
+    <t>Waktu Mulai : 09.00 WIB</t>
+  </si>
+  <si>
+    <t>Waktu Selesai : 08.20 WIB</t>
+  </si>
+  <si>
+    <t>Departure : 08.20 WIB</t>
+  </si>
+  <si>
+    <t>(09.00 - 0.10) - 2.07 = 06.43(JALAN KAKI)</t>
+  </si>
+  <si>
+    <t>(09.00 - 0.10) - 0.22 = 8.28(MOBIL)</t>
+  </si>
+  <si>
+    <t>(09.00 - 0.10) - 0.20 = 8.30(MOTOR)</t>
+  </si>
+  <si>
+    <t>Arrival : 08.50 WIB</t>
+  </si>
+  <si>
+    <t>Waktu Mulai : 18.50 WIB</t>
+  </si>
+  <si>
+    <t>Waktu Mulai : 21.30 WIB</t>
+  </si>
+  <si>
+    <t>Waktu Mulai : 18.00 WIB</t>
+  </si>
+  <si>
+    <t>Waktu Mulai : 19.35 WIB</t>
+  </si>
+  <si>
+    <t>Maleber, KarangTengah, Cianjur(lat:-6.817923 | long:107.175629)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jl. Aceh No. 71 A, Citarum, Bandung Wetan(Lat:-6.9085255 | Long:107.6183885)</t>
+  </si>
+  <si>
+    <t>Jalan Citarum No.23, Citarum, Bandung(Lat:-6.9041041 || Long:107.6221608)</t>
+  </si>
+  <si>
+    <t>Jl. Citarum No.3A, Citarum, Bandung(Lat:-6.9051523 || Long: 107.6212009)</t>
+  </si>
+  <si>
+    <t>Jl. Pajajaran No. 156, Cicendo, Kota Bandung(Lat:-6.9038931 || Long:107.5788389)</t>
+  </si>
+  <si>
+    <t>Jl. Raya Ir. Juanda No.1, Sedati, Sidoarjo, Jawa Timur (Lat:-7.3788851 || Long:112.7872891)</t>
+  </si>
+  <si>
+    <t>Jl. Dukuh Menanggal Sel. No.103 Kota SBY(Lat:-7.3414849 || Long:112.7186495)</t>
+  </si>
+  <si>
+    <t>Jl. Parang Kusumo No.2-I, Kemayoran,  Surabaya(Lat:-7.2397085 || Long:112.7309027)</t>
+  </si>
+  <si>
+    <t>Jl. Parang Kusumo No.2-I, Kemayoran,  Surabaya (Lat:-7.2397085 || Long:112.7309027)</t>
+  </si>
+  <si>
+    <t>Jl. Rajawali No.9-11 Krembangan, Surabaya(Lat:-7.2364681 || Long:112.7367438)</t>
+  </si>
+  <si>
+    <t>Jl. Perintis Kemerdekaan No. 3, Cilaku, Kabupaten Cianjur(Lat:-6.848501 || Long:107.132545)</t>
+  </si>
+  <si>
+    <t>http://www.mapcoordinates.net/en</t>
+  </si>
+  <si>
+    <t>(13.00 - 0.10) -  12.43 = 02.16(JALAN KAKI)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(13.00 - 0.10) - 1.48 = 11.02 (MOBIL) </t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1125,6 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1255,124 +1254,125 @@
     <xf numFmtId="0" fontId="7" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2755,23 +2755,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" topLeftCell="G44" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="49.28515625" customWidth="1"/>
+    <col min="1" max="1" width="57.5703125" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
     <col min="3" max="3" width="50.42578125" customWidth="1"/>
-    <col min="4" max="4" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="86.7109375" customWidth="1"/>
     <col min="5" max="5" width="39.85546875" customWidth="1"/>
-    <col min="6" max="6" width="47.85546875" customWidth="1"/>
+    <col min="6" max="6" width="78.7109375" customWidth="1"/>
     <col min="7" max="7" width="45.85546875" customWidth="1"/>
     <col min="8" max="8" width="47.140625" customWidth="1"/>
     <col min="9" max="9" width="38.5703125" customWidth="1"/>
     <col min="10" max="10" width="43.28515625" customWidth="1"/>
-    <col min="11" max="11" width="53.28515625" customWidth="1"/>
+    <col min="11" max="11" width="78.28515625" customWidth="1"/>
     <col min="12" max="12" width="38.28515625" customWidth="1"/>
     <col min="13" max="13" width="38" customWidth="1"/>
     <col min="14" max="14" width="46.140625" customWidth="1"/>
@@ -2779,72 +2779,75 @@
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>136</v>
+      <c r="A2" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="38" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="50"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="38" t="s">
+        <v>193</v>
+      </c>
+      <c r="E4" s="50"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="39" t="s">
-        <v>119</v>
-      </c>
-      <c r="E3" s="51"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="39" t="s">
-        <v>215</v>
-      </c>
-      <c r="E4" s="51"/>
-    </row>
-    <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" s="39" t="s">
-        <v>120</v>
-      </c>
-      <c r="E5" s="51"/>
+      <c r="B5" s="38" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5" s="50"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="42" t="s">
-        <v>177</v>
-      </c>
-      <c r="B6" s="39" t="s">
-        <v>121</v>
-      </c>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="H6" s="51"/>
+      <c r="A6" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="B6" s="38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="H6" s="50"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
-        <v>182</v>
-      </c>
-      <c r="B7" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="C7" s="43"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="J7" s="51"/>
+      <c r="A7" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="42"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="50"/>
+      <c r="H7" s="50"/>
+      <c r="J7" s="50"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
-        <v>221</v>
-      </c>
-      <c r="E8" s="52"/>
-      <c r="F8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="J8" s="51"/>
+      <c r="A8" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" s="51"/>
+      <c r="F8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="J8" s="50"/>
     </row>
     <row r="9" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
@@ -2852,1283 +2855,1279 @@
         <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="47" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="63" t="s">
-        <v>22</v>
-      </c>
-      <c r="H9" s="61" t="s">
-        <v>41</v>
-      </c>
-      <c r="J9" s="63" t="s">
-        <v>125</v>
-      </c>
-      <c r="K9" s="63" t="s">
-        <v>53</v>
-      </c>
-      <c r="M9" s="58" t="s">
-        <v>126</v>
-      </c>
-      <c r="N9" s="58" t="s">
-        <v>54</v>
+        <v>26</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="K9" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="M9" s="57" t="s">
+        <v>110</v>
+      </c>
+      <c r="N9" s="57" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="99" t="s">
-        <v>12</v>
+      <c r="A10" s="75" t="s">
+        <v>11</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="48" t="s">
-        <v>31</v>
+      <c r="E10" s="47" t="s">
+        <v>28</v>
       </c>
       <c r="G10" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H10" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="M10" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="N10" s="53" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="75"/>
+      <c r="C11" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="H11" s="48" t="s">
+        <v>126</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="M11" s="54" t="s">
+        <v>128</v>
+      </c>
+      <c r="N11" s="54" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="37" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="48" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="K10" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="M10" s="54" t="s">
-        <v>55</v>
-      </c>
-      <c r="N10" s="54" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="99"/>
-      <c r="C11" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="E11" s="49" t="s">
-        <v>141</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="H11" s="49" t="s">
-        <v>142</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="M11" s="55" t="s">
-        <v>144</v>
-      </c>
-      <c r="N11" s="55" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="50" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="50" t="s">
-        <v>43</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="K12" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="M12" s="56" t="s">
-        <v>56</v>
-      </c>
-      <c r="N12" s="56" t="s">
-        <v>61</v>
+      <c r="D12" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="E12" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" s="49" t="s">
+        <v>74</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="M12" s="55" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="55" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="C13" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E13" s="53" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="K13" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="M13" s="57" t="s">
-        <v>60</v>
-      </c>
-      <c r="N13" s="57" t="s">
-        <v>57</v>
+      <c r="C13" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="52" t="s">
+        <v>35</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="M13" s="56" t="s">
+        <v>49</v>
+      </c>
+      <c r="N13" s="56" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C14" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="100"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="10" t="s">
-        <v>11</v>
+      <c r="D14" s="77"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="G14" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="H14" s="77"/>
-      <c r="I14" s="10" t="s">
-        <v>11</v>
+      <c r="H14" s="78"/>
+      <c r="I14" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="J14" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="K14" s="77"/>
-      <c r="L14" s="10" t="s">
-        <v>11</v>
+      <c r="K14" s="78"/>
+      <c r="L14" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="M14" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="N14" s="77"/>
-      <c r="O14" s="59"/>
+      <c r="N14" s="78"/>
+      <c r="O14" s="58"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="78" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="101"/>
-      <c r="E15" s="79"/>
-      <c r="F15" s="14"/>
-      <c r="G15" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="79"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="78" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" s="79"/>
-      <c r="L15" s="14"/>
-      <c r="M15" s="78" t="s">
-        <v>20</v>
-      </c>
-      <c r="N15" s="79"/>
-      <c r="O15" s="59"/>
+        <v>210</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="79" t="s">
+        <v>211</v>
+      </c>
+      <c r="D15" s="80"/>
+      <c r="E15" s="81"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="79" t="s">
+        <v>212</v>
+      </c>
+      <c r="H15" s="81"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="79" t="s">
+        <v>213</v>
+      </c>
+      <c r="K15" s="81"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="79" t="s">
+        <v>211</v>
+      </c>
+      <c r="N15" s="81"/>
+      <c r="O15" s="58"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="B16" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="80" t="s">
-        <v>147</v>
-      </c>
-      <c r="D16" s="102"/>
-      <c r="E16" s="81"/>
-      <c r="F16" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="80" t="s">
-        <v>142</v>
-      </c>
-      <c r="H16" s="81"/>
-      <c r="I16" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="J16" s="82" t="s">
-        <v>142</v>
-      </c>
-      <c r="K16" s="83"/>
-      <c r="L16" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="M16" s="82" t="s">
-        <v>144</v>
-      </c>
-      <c r="N16" s="83"/>
-      <c r="O16" s="59"/>
+      <c r="A16" s="21" t="s">
+        <v>124</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="82" t="s">
+        <v>131</v>
+      </c>
+      <c r="D16" s="83"/>
+      <c r="E16" s="84"/>
+      <c r="F16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="82" t="s">
+        <v>126</v>
+      </c>
+      <c r="H16" s="84"/>
+      <c r="I16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J16" s="85" t="s">
+        <v>126</v>
+      </c>
+      <c r="K16" s="87"/>
+      <c r="L16" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M16" s="85" t="s">
+        <v>128</v>
+      </c>
+      <c r="N16" s="87"/>
+      <c r="O16" s="58"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B17" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" s="82" t="s">
-        <v>157</v>
-      </c>
-      <c r="D17" s="103"/>
-      <c r="E17" s="83"/>
-      <c r="F17" s="13" t="s">
+      <c r="B17" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="85" t="s">
+        <v>141</v>
+      </c>
+      <c r="D17" s="86"/>
+      <c r="E17" s="87"/>
+      <c r="F17" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="85" t="s">
+        <v>183</v>
+      </c>
+      <c r="H17" s="87"/>
+      <c r="I17" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="G17" s="82" t="s">
-        <v>203</v>
-      </c>
-      <c r="H17" s="83"/>
-      <c r="I17" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="J17" s="82" t="s">
-        <v>204</v>
-      </c>
-      <c r="K17" s="83"/>
-      <c r="L17" s="29" t="s">
-        <v>163</v>
-      </c>
-      <c r="M17" s="82" t="s">
-        <v>205</v>
-      </c>
-      <c r="N17" s="83"/>
+      <c r="J17" s="85" t="s">
+        <v>184</v>
+      </c>
+      <c r="K17" s="87"/>
+      <c r="L17" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="M17" s="85" t="s">
+        <v>185</v>
+      </c>
+      <c r="N17" s="87"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="97" t="s">
+        <v>180</v>
+      </c>
+      <c r="D18" s="98"/>
+      <c r="E18" s="99"/>
+      <c r="F18" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="97" t="s">
+        <v>146</v>
+      </c>
+      <c r="H18" s="99"/>
+      <c r="I18" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="J18" s="97" t="s">
+        <v>181</v>
+      </c>
+      <c r="K18" s="99"/>
+      <c r="L18" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="M18" s="97" t="s">
+        <v>186</v>
+      </c>
+      <c r="N18" s="99"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="88" t="s">
+        <v>137</v>
+      </c>
+      <c r="D19" s="89"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" s="104" t="s">
+        <v>140</v>
+      </c>
+      <c r="H19" s="105"/>
+      <c r="I19" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="J19" s="88" t="s">
+        <v>150</v>
+      </c>
+      <c r="K19" s="90"/>
+      <c r="L19" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="M19" s="88" t="s">
+        <v>158</v>
+      </c>
+      <c r="N19" s="90"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B20" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="C20" s="91" t="s">
+        <v>138</v>
+      </c>
+      <c r="D20" s="92"/>
+      <c r="E20" s="93"/>
+      <c r="F20" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" s="91" t="s">
+        <v>144</v>
+      </c>
+      <c r="H20" s="93"/>
+      <c r="I20" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="J20" s="106" t="s">
+        <v>151</v>
+      </c>
+      <c r="K20" s="107"/>
+      <c r="L20" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="M20" s="100" t="s">
+        <v>159</v>
+      </c>
+      <c r="N20" s="101"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="94" t="s">
+        <v>139</v>
+      </c>
+      <c r="D21" s="95"/>
+      <c r="E21" s="96"/>
+      <c r="F21" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="G21" s="102" t="s">
+        <v>145</v>
+      </c>
+      <c r="H21" s="103"/>
+      <c r="I21" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="J21" s="108" t="s">
+        <v>152</v>
+      </c>
+      <c r="K21" s="109"/>
+      <c r="L21" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="M21" s="102" t="s">
+        <v>160</v>
+      </c>
+      <c r="N21" s="103"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="71" t="s">
+        <v>134</v>
+      </c>
+      <c r="B22" s="70" t="s">
         <v>197</v>
       </c>
-      <c r="B18" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="C18" s="84" t="s">
-        <v>198</v>
-      </c>
-      <c r="D18" s="104"/>
-      <c r="E18" s="85"/>
-      <c r="F18" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G18" s="84" t="s">
-        <v>162</v>
-      </c>
-      <c r="H18" s="85"/>
-      <c r="I18" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="J18" s="84" t="s">
-        <v>199</v>
-      </c>
-      <c r="K18" s="85"/>
-      <c r="L18" s="16" t="s">
-        <v>164</v>
-      </c>
-      <c r="M18" s="84" t="s">
-        <v>206</v>
-      </c>
-      <c r="N18" s="85"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="36" t="s">
-        <v>152</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="70" t="s">
-        <v>153</v>
-      </c>
-      <c r="D19" s="96"/>
-      <c r="E19" s="71"/>
-      <c r="F19" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="G19" s="86" t="s">
-        <v>156</v>
-      </c>
-      <c r="H19" s="87"/>
-      <c r="I19" s="28" t="s">
-        <v>159</v>
-      </c>
-      <c r="J19" s="70" t="s">
-        <v>166</v>
-      </c>
-      <c r="K19" s="71"/>
-      <c r="L19" s="28" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
-        <v>148</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="C20" s="88" t="s">
-        <v>154</v>
-      </c>
-      <c r="D20" s="97"/>
-      <c r="E20" s="89"/>
-      <c r="F20" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="G20" s="88" t="s">
-        <v>160</v>
-      </c>
-      <c r="H20" s="89"/>
-      <c r="I20" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="J20" s="72" t="s">
-        <v>167</v>
-      </c>
-      <c r="K20" s="73"/>
-      <c r="L20" s="26" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="40" t="s">
-        <v>149</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="C21" s="92" t="s">
-        <v>155</v>
-      </c>
-      <c r="D21" s="98"/>
-      <c r="E21" s="93"/>
-      <c r="F21" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="G21" s="90" t="s">
-        <v>161</v>
-      </c>
-      <c r="H21" s="91"/>
-      <c r="I21" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="J21" s="74" t="s">
-        <v>168</v>
-      </c>
-      <c r="K21" s="75"/>
-      <c r="L21" s="12" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="109" t="s">
-        <v>150</v>
-      </c>
-      <c r="B22" s="108" t="s">
-        <v>222</v>
-      </c>
-      <c r="C22" s="60"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="60"/>
-      <c r="F22" s="25" t="s">
+      <c r="C22" s="59"/>
+      <c r="D22" s="59"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="H22" s="50"/>
+      <c r="I22" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="L22" s="24" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="43" t="s">
         <v>135</v>
       </c>
-      <c r="H22" s="51"/>
-      <c r="I22" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="L22" s="25" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="44" t="s">
-        <v>151</v>
-      </c>
-      <c r="B23" s="107"/>
+      <c r="B23" s="69"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G24" s="51"/>
-      <c r="H24" s="51"/>
+      <c r="G24" s="50"/>
+      <c r="H24" s="50"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D25" s="51"/>
-      <c r="F25" s="51"/>
-      <c r="G25" s="51"/>
-      <c r="H25" s="51"/>
-      <c r="J25" s="51"/>
+      <c r="D25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="50"/>
+      <c r="H25" s="50"/>
+      <c r="J25" s="50"/>
     </row>
     <row r="26" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B26" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="D26" s="63" t="s">
-        <v>130</v>
-      </c>
-      <c r="F26" s="63" t="s">
-        <v>76</v>
-      </c>
-      <c r="H26" s="63" t="s">
-        <v>78</v>
-      </c>
-      <c r="I26" s="63" t="s">
-        <v>85</v>
-      </c>
-      <c r="K26" s="58" t="s">
-        <v>96</v>
-      </c>
-      <c r="L26" s="58" t="s">
-        <v>108</v>
+        <v>110</v>
+      </c>
+      <c r="B26" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26" s="62" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" s="62" t="s">
+        <v>65</v>
+      </c>
+      <c r="H26" s="62" t="s">
+        <v>67</v>
+      </c>
+      <c r="I26" s="62" t="s">
+        <v>73</v>
+      </c>
+      <c r="K26" s="57" t="s">
+        <v>83</v>
+      </c>
+      <c r="L26" s="57" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="K27" s="54" t="s">
-        <v>47</v>
-      </c>
-      <c r="L27" s="54" t="s">
-        <v>91</v>
+        <v>34</v>
+      </c>
+      <c r="K27" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="L27" s="53" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="K28" s="55" t="s">
-        <v>143</v>
-      </c>
-      <c r="L28" s="55" t="s">
-        <v>143</v>
+        <v>127</v>
+      </c>
+      <c r="K28" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="L28" s="54" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="B29" s="23" t="s">
+      <c r="A29" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F29" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="F29" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="H29" s="23" t="s">
+      <c r="H29" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="I29" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="K29" s="55" t="s">
+        <v>39</v>
+      </c>
+      <c r="L29" s="55" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" s="23" t="s">
+        <v>200</v>
+      </c>
+      <c r="H30" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="K30" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="I29" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="K29" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="L29" s="56" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="F30" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="H30" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="I30" s="24" t="s">
-        <v>44</v>
-      </c>
-      <c r="K30" s="57" t="s">
-        <v>92</v>
-      </c>
-      <c r="L30" s="57" t="s">
-        <v>52</v>
+      <c r="L30" s="56" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A31" s="76" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="77"/>
-      <c r="C31" s="10" t="s">
-        <v>11</v>
+      <c r="B31" s="78"/>
+      <c r="C31" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>11</v>
+        <v>51</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="F31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31" s="76" t="s">
+        <v>66</v>
+      </c>
+      <c r="I31" s="78"/>
+      <c r="J31" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K31" s="76" t="s">
+        <v>72</v>
+      </c>
+      <c r="L31" s="78"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="79" t="s">
+        <v>211</v>
+      </c>
+      <c r="B32" s="81"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="E32" s="13"/>
+      <c r="F32" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G32" s="13"/>
+      <c r="H32" s="79" t="s">
+        <v>216</v>
+      </c>
+      <c r="I32" s="81"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="79" t="s">
+        <v>217</v>
+      </c>
+      <c r="L32" s="81"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="85" t="s">
+        <v>128</v>
+      </c>
+      <c r="B33" s="87"/>
+      <c r="C33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="82" t="s">
+        <v>127</v>
+      </c>
+      <c r="I33" s="84"/>
+      <c r="J33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K33" s="85" t="s">
+        <v>127</v>
+      </c>
+      <c r="L33" s="87"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="85" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="87"/>
+      <c r="C34" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="D34" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="F34" s="21" t="s">
+        <v>166</v>
+      </c>
+      <c r="G34" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" s="85" t="s">
+        <v>205</v>
+      </c>
+      <c r="I34" s="87"/>
+      <c r="J34" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="K34" s="85" t="s">
+        <v>184</v>
+      </c>
+      <c r="L34" s="87"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="97" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35" s="99"/>
+      <c r="C35" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="D35" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="E35" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="G31" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="H31" s="76" t="s">
-        <v>77</v>
-      </c>
-      <c r="I31" s="77"/>
-      <c r="J31" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K31" s="76" t="s">
-        <v>84</v>
-      </c>
-      <c r="L31" s="77"/>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="78" t="s">
-        <v>20</v>
-      </c>
-      <c r="B32" s="79"/>
-      <c r="C32" s="14"/>
-      <c r="D32" s="3" t="s">
+      <c r="F35" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="G35" s="30" t="s">
+        <v>162</v>
+      </c>
+      <c r="H35" s="97" t="s">
+        <v>75</v>
+      </c>
+      <c r="I35" s="99"/>
+      <c r="J35" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="K35" s="97" t="s">
+        <v>188</v>
+      </c>
+      <c r="L35" s="99"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="88" t="s">
+        <v>158</v>
+      </c>
+      <c r="B36" s="90"/>
+      <c r="C36" s="27" t="s">
+        <v>155</v>
+      </c>
+      <c r="D36" s="68" t="s">
+        <v>55</v>
+      </c>
+      <c r="E36" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="F36" s="44" t="s">
+        <v>202</v>
+      </c>
+      <c r="G36" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="H36" s="91" t="s">
+        <v>165</v>
+      </c>
+      <c r="I36" s="93"/>
+      <c r="J36" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="K36" s="88" t="s">
+        <v>170</v>
+      </c>
+      <c r="L36" s="90"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="100" t="s">
+        <v>159</v>
+      </c>
+      <c r="B37" s="101"/>
+      <c r="C37" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="D37" s="67" t="s">
+        <v>194</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="F37" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="G37" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="H37" s="91" t="s">
+        <v>167</v>
+      </c>
+      <c r="I37" s="93"/>
+      <c r="J37" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="K37" s="91" t="s">
+        <v>171</v>
+      </c>
+      <c r="L37" s="93"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="102" t="s">
+        <v>160</v>
+      </c>
+      <c r="B38" s="103"/>
+      <c r="C38" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D38" s="64" t="s">
+        <v>127</v>
+      </c>
+      <c r="E38" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="E32" s="14"/>
-      <c r="F32" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G32" s="14"/>
-      <c r="H32" s="78" t="s">
-        <v>107</v>
-      </c>
-      <c r="I32" s="79"/>
-      <c r="J32" s="14"/>
-      <c r="K32" s="78" t="s">
-        <v>88</v>
-      </c>
-      <c r="L32" s="79"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="82" t="s">
-        <v>144</v>
-      </c>
-      <c r="B33" s="83"/>
-      <c r="C33" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D33" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="G33" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="80" t="s">
-        <v>143</v>
-      </c>
-      <c r="I33" s="81"/>
-      <c r="J33" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="K33" s="82" t="s">
-        <v>143</v>
-      </c>
-      <c r="L33" s="83"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="82" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="83"/>
-      <c r="C34" s="29" t="s">
+      <c r="F38" s="43" t="s">
+        <v>204</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="H38" s="94" t="s">
         <v>169</v>
       </c>
-      <c r="D34" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="E34" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="F34" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="G34" s="33" t="s">
-        <v>80</v>
-      </c>
-      <c r="H34" s="82" t="s">
-        <v>208</v>
-      </c>
-      <c r="I34" s="83"/>
-      <c r="J34" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="K34" s="82" t="s">
-        <v>204</v>
-      </c>
-      <c r="L34" s="83"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="84" t="s">
-        <v>200</v>
-      </c>
-      <c r="B35" s="85"/>
-      <c r="C35" s="16" t="s">
-        <v>170</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="F35" s="21" t="s">
-        <v>202</v>
-      </c>
-      <c r="G35" s="31" t="s">
-        <v>178</v>
-      </c>
-      <c r="H35" s="84" t="s">
-        <v>87</v>
-      </c>
-      <c r="I35" s="85"/>
-      <c r="J35" s="34" t="s">
-        <v>129</v>
-      </c>
-      <c r="K35" s="84" t="s">
-        <v>210</v>
-      </c>
-      <c r="L35" s="85"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="70" t="s">
-        <v>174</v>
-      </c>
-      <c r="B36" s="71"/>
-      <c r="C36" s="28" t="s">
-        <v>171</v>
-      </c>
-      <c r="D36" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="E36" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="F36" s="45" t="s">
-        <v>180</v>
-      </c>
-      <c r="G36" s="35" t="s">
-        <v>181</v>
-      </c>
-      <c r="H36" s="88" t="s">
-        <v>183</v>
-      </c>
-      <c r="I36" s="89"/>
-      <c r="J36" s="46" t="s">
-        <v>186</v>
-      </c>
-      <c r="K36" s="70" t="s">
-        <v>188</v>
-      </c>
-      <c r="L36" s="71"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="94" t="s">
-        <v>175</v>
-      </c>
-      <c r="B37" s="95"/>
-      <c r="C37" s="26" t="s">
-        <v>218</v>
-      </c>
-      <c r="D37" s="68" t="s">
-        <v>216</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="F37" s="41" t="s">
-        <v>179</v>
-      </c>
-      <c r="G37" s="34" t="s">
-        <v>81</v>
-      </c>
-      <c r="H37" s="88" t="s">
-        <v>185</v>
-      </c>
-      <c r="I37" s="89"/>
-      <c r="J37" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K37" s="88" t="s">
-        <v>189</v>
-      </c>
-      <c r="L37" s="89"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="90" t="s">
-        <v>176</v>
-      </c>
-      <c r="B38" s="91"/>
-      <c r="C38" s="12" t="s">
-        <v>219</v>
-      </c>
-      <c r="D38" s="65" t="s">
-        <v>143</v>
-      </c>
-      <c r="E38" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="F38" s="44" t="s">
-        <v>201</v>
-      </c>
-      <c r="G38" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="H38" s="92" t="s">
-        <v>187</v>
-      </c>
-      <c r="I38" s="93"/>
-      <c r="J38" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="K38" s="92" t="s">
-        <v>191</v>
-      </c>
-      <c r="L38" s="93"/>
+      <c r="I38" s="96"/>
+      <c r="J38" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="K38" s="94" t="s">
+        <v>173</v>
+      </c>
+      <c r="L38" s="96"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C39" s="25" t="s">
-        <v>220</v>
-      </c>
-      <c r="D39" s="66" t="s">
-        <v>67</v>
-      </c>
-      <c r="E39" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="F39" s="51"/>
-      <c r="G39" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="H39" s="51"/>
-      <c r="J39" s="25" t="s">
-        <v>39</v>
+      <c r="C39" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" s="50"/>
+      <c r="G39" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="H39" s="50"/>
+      <c r="J39" s="24" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D40" s="67" t="s">
-        <v>68</v>
-      </c>
-      <c r="F40" s="51"/>
-      <c r="H40" s="51"/>
+      <c r="D40" s="66" t="s">
+        <v>57</v>
+      </c>
+      <c r="F40" s="50"/>
+      <c r="H40" s="50"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D41" s="51"/>
-      <c r="J41" s="51"/>
+      <c r="D41" s="50"/>
+      <c r="J41" s="50"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D42" s="51"/>
+      <c r="D42" s="50"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D43" s="51"/>
-      <c r="F43" s="51"/>
-      <c r="H43" s="51"/>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51"/>
+      <c r="D43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="H43" s="50"/>
+      <c r="I43" s="50"/>
+      <c r="J43" s="50"/>
     </row>
     <row r="44" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B44" s="63" t="s">
-        <v>108</v>
-      </c>
-      <c r="D44" s="63" t="s">
-        <v>109</v>
-      </c>
-      <c r="E44" s="63" t="s">
-        <v>138</v>
-      </c>
-      <c r="G44" s="63" t="s">
-        <v>110</v>
-      </c>
-      <c r="I44" s="63" t="s">
-        <v>113</v>
-      </c>
-      <c r="K44" s="63" t="s">
-        <v>139</v>
+        <v>83</v>
+      </c>
+      <c r="B44" s="62" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" s="62" t="s">
+        <v>94</v>
+      </c>
+      <c r="E44" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="G44" s="62" t="s">
+        <v>95</v>
+      </c>
+      <c r="I44" s="62" t="s">
+        <v>97</v>
+      </c>
+      <c r="K44" s="62" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A47" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="D47" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="E47" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="G47" s="23" t="s">
-        <v>72</v>
-      </c>
-      <c r="I47" s="23" t="s">
-        <v>172</v>
-      </c>
-      <c r="K47" s="23" t="s">
+      <c r="A47" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>80</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="I47" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="K47" s="22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D48" s="23" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="24" t="s">
+      <c r="E48" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="G48" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="B48" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D48" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="E48" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="G48" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="I48" s="24" t="s">
-        <v>173</v>
-      </c>
-      <c r="K48" s="24" t="s">
-        <v>118</v>
+      <c r="I48" s="23" t="s">
+        <v>157</v>
+      </c>
+      <c r="K48" s="23" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A49" s="76" t="s">
-        <v>84</v>
-      </c>
-      <c r="B49" s="77"/>
-      <c r="C49" s="10" t="s">
-        <v>11</v>
+        <v>72</v>
+      </c>
+      <c r="B49" s="78"/>
+      <c r="C49" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="D49" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="E49" s="77"/>
-      <c r="F49" s="10" t="s">
-        <v>11</v>
+      <c r="E49" s="78"/>
+      <c r="F49" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="G49" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J49" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" s="79" t="s">
+        <v>218</v>
+      </c>
+      <c r="B50" s="81"/>
+      <c r="C50" s="13"/>
+      <c r="D50" s="79" t="s">
+        <v>219</v>
+      </c>
+      <c r="E50" s="81"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H50" s="13"/>
+      <c r="I50" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="J50" s="13"/>
+      <c r="K50" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="85" t="s">
+        <v>127</v>
+      </c>
+      <c r="B51" s="87"/>
+      <c r="C51" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" s="85" t="s">
+        <v>129</v>
+      </c>
+      <c r="E51" s="87"/>
+      <c r="F51" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="H51" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="I51" s="35" t="s">
+        <v>130</v>
+      </c>
+      <c r="J51" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K51" s="35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="85" t="s">
+        <v>77</v>
+      </c>
+      <c r="B52" s="87"/>
+      <c r="C52" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="D52" s="85" t="s">
+        <v>189</v>
+      </c>
+      <c r="E52" s="87"/>
+      <c r="F52" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="G52" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="H52" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="I52" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="J52" s="11" t="s">
+        <v>192</v>
+      </c>
+      <c r="K52" s="21" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="85" t="s">
+        <v>188</v>
+      </c>
+      <c r="B53" s="87"/>
+      <c r="C53" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" s="97" t="s">
+        <v>190</v>
+      </c>
+      <c r="E53" s="99"/>
+      <c r="F53" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="G53" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H53" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="H49" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="J49" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="K49" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="78" t="s">
+      <c r="I53" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="J53" s="15" t="s">
+        <v>191</v>
+      </c>
+      <c r="K53" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="88" t="s">
+        <v>170</v>
+      </c>
+      <c r="B54" s="90"/>
+      <c r="C54" s="26" t="s">
+        <v>172</v>
+      </c>
+      <c r="D54" s="88" t="s">
+        <v>176</v>
+      </c>
+      <c r="E54" s="90"/>
+      <c r="F54" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="G54" s="68" t="s">
+        <v>55</v>
+      </c>
+      <c r="H54" s="31" t="s">
+        <v>71</v>
+      </c>
+      <c r="I54" s="39" t="s">
+        <v>222</v>
+      </c>
+      <c r="J54" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="K54" s="73" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="91" t="s">
+        <v>171</v>
+      </c>
+      <c r="B55" s="93"/>
+      <c r="C55" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="D55" s="100" t="s">
+        <v>177</v>
+      </c>
+      <c r="E55" s="101"/>
+      <c r="F55" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="G55" s="63" t="s">
+        <v>195</v>
+      </c>
+      <c r="H55" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="I55" s="39" t="s">
+        <v>223</v>
+      </c>
+      <c r="J55" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="K55" s="74"/>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A56" s="94" t="s">
+        <v>173</v>
+      </c>
+      <c r="B56" s="96"/>
+      <c r="C56" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D56" s="102" t="s">
+        <v>178</v>
+      </c>
+      <c r="E56" s="103"/>
+      <c r="F56" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="G56" s="64" t="s">
+        <v>130</v>
+      </c>
+      <c r="H56" s="30" t="s">
+        <v>63</v>
+      </c>
+      <c r="J56" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="K56" s="61" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C57" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="D57" s="50"/>
+      <c r="F57" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="G57" s="65" t="s">
         <v>88</v>
       </c>
-      <c r="B50" s="79"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="78" t="s">
-        <v>97</v>
-      </c>
-      <c r="E50" s="79"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="H50" s="14"/>
-      <c r="I50" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="J50" s="14"/>
-      <c r="K50" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="82" t="s">
-        <v>143</v>
-      </c>
-      <c r="B51" s="83"/>
-      <c r="C51" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" s="82" t="s">
-        <v>145</v>
-      </c>
-      <c r="E51" s="83"/>
-      <c r="F51" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G51" s="36" t="s">
-        <v>146</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="I51" s="36" t="s">
-        <v>146</v>
-      </c>
-      <c r="J51" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="K51" s="36" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="82" t="s">
-        <v>90</v>
-      </c>
-      <c r="B52" s="83"/>
-      <c r="C52" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="D52" s="82" t="s">
-        <v>211</v>
-      </c>
-      <c r="E52" s="83"/>
-      <c r="F52" s="29" t="s">
-        <v>193</v>
-      </c>
-      <c r="G52" s="22" t="s">
-        <v>104</v>
-      </c>
-      <c r="H52" s="30" t="s">
-        <v>69</v>
-      </c>
-      <c r="I52" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="J52" s="12" t="s">
-        <v>214</v>
-      </c>
-      <c r="K52" s="22" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="82" t="s">
-        <v>210</v>
-      </c>
-      <c r="B53" s="83"/>
-      <c r="C53" s="29" t="s">
-        <v>95</v>
-      </c>
-      <c r="D53" s="84" t="s">
-        <v>212</v>
-      </c>
-      <c r="E53" s="85"/>
-      <c r="F53" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="G53" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="H53" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="I53" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="J53" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="K53" s="21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="70" t="s">
-        <v>188</v>
-      </c>
-      <c r="B54" s="71"/>
-      <c r="C54" s="27" t="s">
-        <v>190</v>
-      </c>
-      <c r="D54" s="70" t="s">
-        <v>194</v>
-      </c>
-      <c r="E54" s="71"/>
-      <c r="F54" s="28" t="s">
-        <v>101</v>
-      </c>
-      <c r="G54" s="69" t="s">
-        <v>66</v>
-      </c>
-      <c r="H54" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="J54" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="K54" s="106" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="88" t="s">
-        <v>189</v>
-      </c>
-      <c r="B55" s="89"/>
-      <c r="C55" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D55" s="94" t="s">
-        <v>195</v>
-      </c>
-      <c r="E55" s="95"/>
-      <c r="F55" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="G55" s="64" t="s">
-        <v>217</v>
-      </c>
-      <c r="H55" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="J55" s="26" t="s">
-        <v>37</v>
-      </c>
-      <c r="K55" s="105"/>
-    </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="92" t="s">
-        <v>191</v>
-      </c>
-      <c r="B56" s="93"/>
-      <c r="C56" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="D56" s="90" t="s">
-        <v>196</v>
-      </c>
-      <c r="E56" s="91"/>
-      <c r="F56" s="12" t="s">
-        <v>134</v>
-      </c>
-      <c r="G56" s="65" t="s">
-        <v>146</v>
-      </c>
-      <c r="H56" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="J56" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="K56" s="62" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C57" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="D57" s="51"/>
-      <c r="F57" s="25" t="s">
-        <v>135</v>
-      </c>
-      <c r="G57" s="66" t="s">
-        <v>102</v>
-      </c>
-      <c r="H57" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="J57" s="25" t="s">
-        <v>39</v>
-      </c>
-      <c r="K57" s="51"/>
+      <c r="H57" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="J57" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="K57" s="50"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D58" s="51"/>
-      <c r="G58" s="67" t="s">
-        <v>103</v>
-      </c>
-      <c r="H58" s="51"/>
-      <c r="I58" s="51"/>
-      <c r="J58" s="51"/>
+      <c r="D58" s="50"/>
+      <c r="G58" s="66" t="s">
+        <v>89</v>
+      </c>
+      <c r="H58" s="50"/>
+      <c r="I58" s="50"/>
+      <c r="J58" s="50"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F59" s="51"/>
+      <c r="F59" s="50"/>
     </row>
   </sheetData>
-  <mergeCells count="71">
-    <mergeCell ref="K54:K55"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
+  <mergeCells count="74">
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
     <mergeCell ref="A56:B56"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="D50:E50"/>
@@ -4143,22 +4142,47 @@
     <mergeCell ref="A53:B53"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A55:B55"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="K54:K55"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A36:B36"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{22769755-18A0-4228-9384-568445F69ECC}"/>
@@ -4166,9 +4190,10 @@
     <hyperlink ref="B6" r:id="rId3" xr:uid="{77F85450-50CF-45C9-8D04-92B93616F32E}"/>
     <hyperlink ref="B7" r:id="rId4" xr:uid="{C8FB0067-ED59-4BC0-8C56-F67274EB48A8}"/>
     <hyperlink ref="B4" r:id="rId5" xr:uid="{DFEC60C0-6336-4B8F-A83F-DC250E52EDE6}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{EC28AFA3-8E64-4B66-A9DA-F5A51E377CE6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId6"/>
-  <drawing r:id="rId7"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>
+  <drawing r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
penambahan moda yg tidak memungkinkan dari hasil review dan perapihan
</commit_message>
<xml_diff>
--- a/Documents/DIAGRAM STUDI KASUS V.4.1.xlsx
+++ b/Documents/DIAGRAM STUDI KASUS V.4.1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="231">
   <si>
     <t>Arrival : -</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Jalan Kaki(1Km, 15 menit)</t>
   </si>
   <si>
-    <t>Jalan Kaki(77.85Km, 740 menit)</t>
-  </si>
-  <si>
     <t>EVENT [2.1]</t>
   </si>
   <si>
@@ -189,9 +186,6 @@
     <t>EVENT :  CHECK IN(KTP,TIKET,KLARIFIKASI)</t>
   </si>
   <si>
-    <t>Waktu Mulai : 05.20 WIB</t>
-  </si>
-  <si>
     <t>JADWAL KEBERANGKATAN PESAWAT</t>
   </si>
   <si>
@@ -201,9 +195,6 @@
     <t>Waktu Tiba : 07:15 (SUB)</t>
   </si>
   <si>
-    <t>Jalan Kaki(648 Km, 7980 menit)</t>
-  </si>
-  <si>
     <t>BANDARA JUANDA SURABAYA</t>
   </si>
   <si>
@@ -219,9 +210,6 @@
     <t>Pesawat(578KM,75menit)</t>
   </si>
   <si>
-    <t>kereta api(699 Km,720 menit)</t>
-  </si>
-  <si>
     <t>EVENT [6]</t>
   </si>
   <si>
@@ -231,18 +219,9 @@
     <t>EVENT [7]</t>
   </si>
   <si>
-    <t>Jalan Kaki(10.3 Km, 127 menit)</t>
-  </si>
-  <si>
     <t>Bus(15.7 Km, 38 menit)</t>
   </si>
   <si>
-    <t>Mobil(781 Km,856 menit)</t>
-  </si>
-  <si>
-    <t>Motor(624 Km, 600 menit)</t>
-  </si>
-  <si>
     <t>BEBEK HANDAYANI SURABAYA</t>
   </si>
   <si>
@@ -255,9 +234,6 @@
     <t>Departure : 15.25 WIB</t>
   </si>
   <si>
-    <t>Jalan Kaki(13.6 Km, 170 menit)</t>
-  </si>
-  <si>
     <t>Arrival : 15.55 WIB</t>
   </si>
   <si>
@@ -295,9 +271,6 @@
   </si>
   <si>
     <t>Waktu Tiba : 09:20 (BDO)</t>
-  </si>
-  <si>
-    <t>Arrival : 07.10 WIB</t>
   </si>
   <si>
     <t>Departure : 08.05 WIB</t>
@@ -491,9 +464,6 @@
     <t>Jalan Kaki(0.6Km, 7 menit)</t>
   </si>
   <si>
-    <t>Mobil(0.65Km, 2 menit)</t>
-  </si>
-  <si>
     <t>Motor(0.65Km, 1 menit)</t>
   </si>
   <si>
@@ -506,12 +476,6 @@
     <t>(21.00 - 0.10) - 0.1 = 20.49(MOTOR)</t>
   </si>
   <si>
-    <t>Jalan Kaki(4.6Km,58 menit)</t>
-  </si>
-  <si>
-    <t>Mobil'umum'(6.0Km,16 menit)</t>
-  </si>
-  <si>
     <t>Motor(6.0Km, 14 menit)</t>
   </si>
   <si>
@@ -563,9 +527,6 @@
     <t>(19.30 - 0.10) - 0.3 = 19.17(MOBIL)</t>
   </si>
   <si>
-    <t>Motor'umum'(1.2 km, 2menit)</t>
-  </si>
-  <si>
     <t>(19.30 - 0.10) - 0.2 = 19.18(MOTOR)</t>
   </si>
   <si>
@@ -575,15 +536,6 @@
     <t>Jalan Kaki(20.3Km, 252 menit)</t>
   </si>
   <si>
-    <t>(07.20 - 0.10) - 4.12 = 02.38(JALAN KAKI)</t>
-  </si>
-  <si>
-    <t>(07.20 - 0.10) - 0.37 = 06.33(MOBIL)</t>
-  </si>
-  <si>
-    <t>(07.20 - 0.10) - 0.32 = 07.38(MOTOR)</t>
-  </si>
-  <si>
     <t>Departure : 16.15 WIB</t>
   </si>
   <si>
@@ -593,9 +545,6 @@
     <t>Departure : 20.48 WIB</t>
   </si>
   <si>
-    <t>Departure : 04.54 WIB</t>
-  </si>
-  <si>
     <t>Arrival : 06.50 WIB</t>
   </si>
   <si>
@@ -608,24 +557,15 @@
     <t>Departure : 04.54WIB</t>
   </si>
   <si>
-    <t>Arrival : 05.10 WIB</t>
-  </si>
-  <si>
     <t>Departure : 19.18 WIB</t>
   </si>
   <si>
     <t>Arrival : 19.20 WIB</t>
   </si>
   <si>
-    <t>Departure : 06.33 WIB</t>
-  </si>
-  <si>
     <t>Mobil'dinas'(67.4 Km, 108 menit)</t>
   </si>
   <si>
-    <t>Jalan Kaki(60.7 Km, 746 menit)</t>
-  </si>
-  <si>
     <t xml:space="preserve">www.skyscanner.com </t>
   </si>
   <si>
@@ -717,12 +657,286 @@
   </si>
   <si>
     <t xml:space="preserve">(13.00 - 0.10) - 1.48 = 11.02 (MOBIL) </t>
+  </si>
+  <si>
+    <t>Mobil'angkot'(0.65Km, 2 menit)</t>
+  </si>
+  <si>
+    <t>Mobil'Taxi'(6.0Km,16 menit)</t>
+  </si>
+  <si>
+    <t>Motor'angkot'(1.2 km, 2menit)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Jalan Kaki(648 Km, 7980 menit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tidak memungkinkan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mobil(781 Km,856 menit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tidak memungkinkan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Motor(624 Km, 600 menit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tidak memungkinkan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Departure : 04.33 WIB</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Jalan Kaki(77.85Km, 740 menit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tidak memungkinkan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Waktu Mulai : 06.20 WIB</t>
+  </si>
+  <si>
+    <t>Arrival : 06.10 WIB</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">kereta api(699 Km,720 menit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tidak memungkinkan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Jalan Kaki(4.6Km,58 menit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tidak memungkinkan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Waktu Mulai : 04.20 WIB</t>
+  </si>
+  <si>
+    <t>Waktu Selesai : 03.40 WIB</t>
+  </si>
+  <si>
+    <t>Waktu Mulai : 03.40 WIB</t>
+  </si>
+  <si>
+    <t>Departure : 04.00 WIB</t>
+  </si>
+  <si>
+    <t>Waktu Selesai : 03.45 WIB</t>
+  </si>
+  <si>
+    <t>(04.20 - 0.10) - 0.16 = 03.54(MOBIL)</t>
+  </si>
+  <si>
+    <t>Arrival : 04.10 WIB</t>
+  </si>
+  <si>
+    <t>(04.20 - 0.10) - 0.14 = 03.56(MOTOR)</t>
+  </si>
+  <si>
+    <t>(04.20 - 0.10) - 0.58 = 03.18(JALAN KAKI)</t>
+  </si>
+  <si>
+    <t>(06.20 - 0.10) - 4.12 = 01.38(JALAN KAKI)</t>
+  </si>
+  <si>
+    <t>(06.20 - 0.10) - 0.37 = 05.33(MOBIL)</t>
+  </si>
+  <si>
+    <t>(06.20 - 0.10) - 0.32 = 05.38(MOTOR)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Jalan Kaki(60.7 Km, 746 menit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tidak memungkinkan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Jalan Kaki(10.3 Km, 127 menit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tidak memungkinkan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Jalan Kaki(13.6 Km, 170 menit </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tidak memungkinkan</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1106,7 +1320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1179,9 +1393,6 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1257,120 +1468,120 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2752,11 +2963,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G27" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2765,12 +2976,12 @@
     <col min="2" max="2" width="51" customWidth="1"/>
     <col min="3" max="3" width="50.42578125" customWidth="1"/>
     <col min="4" max="4" width="86.7109375" customWidth="1"/>
-    <col min="5" max="5" width="39.85546875" customWidth="1"/>
+    <col min="5" max="5" width="45.42578125" customWidth="1"/>
     <col min="6" max="6" width="78.7109375" customWidth="1"/>
-    <col min="7" max="7" width="45.85546875" customWidth="1"/>
+    <col min="7" max="7" width="49" customWidth="1"/>
     <col min="8" max="8" width="47.140625" customWidth="1"/>
     <col min="9" max="9" width="38.5703125" customWidth="1"/>
-    <col min="10" max="10" width="43.28515625" customWidth="1"/>
+    <col min="10" max="10" width="49.85546875" customWidth="1"/>
     <col min="11" max="11" width="78.28515625" customWidth="1"/>
     <col min="12" max="12" width="38.28515625" customWidth="1"/>
     <col min="13" max="13" width="38" customWidth="1"/>
@@ -2780,74 +2991,74 @@
     <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>120</v>
+        <v>112</v>
+      </c>
+      <c r="B2" s="35" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="38" t="s">
-        <v>103</v>
-      </c>
-      <c r="E3" s="50"/>
+      <c r="B3" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="49"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="38" t="s">
-        <v>193</v>
-      </c>
-      <c r="E4" s="50"/>
+      <c r="B4" s="37" t="s">
+        <v>173</v>
+      </c>
+      <c r="E4" s="49"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="38" t="s">
-        <v>104</v>
-      </c>
-      <c r="E5" s="50"/>
+      <c r="B5" s="37" t="s">
+        <v>95</v>
+      </c>
+      <c r="E5" s="49"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="41" t="s">
-        <v>161</v>
-      </c>
-      <c r="B6" s="38" t="s">
-        <v>105</v>
-      </c>
-      <c r="C6" s="72" t="s">
-        <v>221</v>
-      </c>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="H6" s="50"/>
+      <c r="A6" s="40" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="70" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="H6" s="49"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
-        <v>164</v>
-      </c>
-      <c r="B7" s="42" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="42"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="50"/>
-      <c r="H7" s="50"/>
-      <c r="J7" s="50"/>
+      <c r="A7" s="40" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="41"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="J7" s="49"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="41" t="s">
-        <v>196</v>
-      </c>
-      <c r="E8" s="51"/>
-      <c r="F8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="J8" s="50"/>
+      <c r="A8" s="40" t="s">
+        <v>176</v>
+      </c>
+      <c r="E8" s="50"/>
+      <c r="F8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="J8" s="49"/>
     </row>
     <row r="9" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
@@ -2857,30 +3068,30 @@
       <c r="D9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="62" t="s">
+      <c r="G9" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="H9" s="60" t="s">
-        <v>33</v>
-      </c>
-      <c r="J9" s="62" t="s">
-        <v>109</v>
-      </c>
-      <c r="K9" s="62" t="s">
+      <c r="H9" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="61" t="s">
+        <v>100</v>
+      </c>
+      <c r="K9" s="61" t="s">
+        <v>41</v>
+      </c>
+      <c r="M9" s="56" t="s">
+        <v>101</v>
+      </c>
+      <c r="N9" s="56" t="s">
         <v>42</v>
       </c>
-      <c r="M9" s="57" t="s">
-        <v>110</v>
-      </c>
-      <c r="N9" s="57" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="73" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -2889,88 +3100,88 @@
       <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="47" t="s">
+      <c r="E10" s="46" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="47" t="s">
-        <v>34</v>
+      <c r="H10" s="46" t="s">
+        <v>33</v>
       </c>
       <c r="J10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="M10" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="N10" s="53" t="s">
-        <v>47</v>
+      <c r="M10" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="N10" s="52" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="101"/>
+      <c r="A11" s="73"/>
       <c r="C11" s="7" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="E11" s="48" t="s">
-        <v>125</v>
+        <v>115</v>
+      </c>
+      <c r="E11" s="47" t="s">
+        <v>116</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="H11" s="48" t="s">
-        <v>126</v>
+        <v>117</v>
+      </c>
+      <c r="H11" s="47" t="s">
+        <v>117</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="K11" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="M11" s="54" t="s">
-        <v>128</v>
-      </c>
-      <c r="N11" s="54" t="s">
-        <v>127</v>
+        <v>117</v>
+      </c>
+      <c r="M11" s="53" t="s">
+        <v>119</v>
+      </c>
+      <c r="N11" s="53" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="37" t="s">
-        <v>108</v>
+      <c r="A12" s="36" t="s">
+        <v>99</v>
       </c>
       <c r="C12" s="22" t="s">
         <v>23</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="E12" s="49" t="s">
-        <v>207</v>
+        <v>186</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>187</v>
       </c>
       <c r="G12" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="H12" s="49" t="s">
-        <v>74</v>
+      <c r="H12" s="48" t="s">
+        <v>67</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="M12" s="55" t="s">
-        <v>45</v>
-      </c>
-      <c r="N12" s="55" t="s">
-        <v>50</v>
+        <v>188</v>
+      </c>
+      <c r="M12" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="N12" s="54" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
@@ -2981,26 +3192,26 @@
       <c r="D13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="52" t="s">
+      <c r="E13" s="51" t="s">
         <v>29</v>
       </c>
       <c r="G13" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="H13" s="52" t="s">
-        <v>35</v>
+      <c r="H13" s="51" t="s">
+        <v>34</v>
       </c>
       <c r="J13" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="K13" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="M13" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="N13" s="56" t="s">
-        <v>46</v>
+      <c r="M13" s="55" t="s">
+        <v>48</v>
+      </c>
+      <c r="N13" s="55" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="18.75" x14ac:dyDescent="0.25">
@@ -3010,1105 +3221,1163 @@
       <c r="B14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="87" t="s">
+      <c r="C14" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="D14" s="102"/>
-      <c r="E14" s="88"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="76"/>
       <c r="F14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="87" t="s">
+      <c r="G14" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="H14" s="88"/>
+      <c r="H14" s="76"/>
       <c r="I14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="J14" s="87" t="s">
+      <c r="J14" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="K14" s="88"/>
+      <c r="K14" s="76"/>
       <c r="L14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="M14" s="87" t="s">
+      <c r="M14" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="N14" s="88"/>
-      <c r="O14" s="58"/>
+      <c r="N14" s="76"/>
+      <c r="O14" s="57"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>210</v>
+        <v>190</v>
       </c>
       <c r="B15" s="13"/>
-      <c r="C15" s="89" t="s">
-        <v>211</v>
-      </c>
-      <c r="D15" s="103"/>
-      <c r="E15" s="90"/>
+      <c r="C15" s="77" t="s">
+        <v>191</v>
+      </c>
+      <c r="D15" s="78"/>
+      <c r="E15" s="79"/>
       <c r="F15" s="13"/>
-      <c r="G15" s="89" t="s">
-        <v>212</v>
-      </c>
-      <c r="H15" s="90"/>
+      <c r="G15" s="77" t="s">
+        <v>192</v>
+      </c>
+      <c r="H15" s="79"/>
       <c r="I15" s="13"/>
-      <c r="J15" s="89" t="s">
-        <v>213</v>
-      </c>
-      <c r="K15" s="90"/>
+      <c r="J15" s="77" t="s">
+        <v>193</v>
+      </c>
+      <c r="K15" s="79"/>
       <c r="L15" s="13"/>
-      <c r="M15" s="89" t="s">
-        <v>211</v>
-      </c>
-      <c r="N15" s="90"/>
-      <c r="O15" s="58"/>
+      <c r="M15" s="77" t="s">
+        <v>191</v>
+      </c>
+      <c r="N15" s="79"/>
+      <c r="O15" s="57"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="95" t="s">
-        <v>131</v>
-      </c>
-      <c r="D16" s="104"/>
-      <c r="E16" s="96"/>
+      <c r="C16" s="80" t="s">
+        <v>122</v>
+      </c>
+      <c r="D16" s="81"/>
+      <c r="E16" s="82"/>
       <c r="F16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="95" t="s">
-        <v>126</v>
-      </c>
-      <c r="H16" s="96"/>
+      <c r="G16" s="80" t="s">
+        <v>117</v>
+      </c>
+      <c r="H16" s="82"/>
       <c r="I16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="J16" s="91" t="s">
-        <v>126</v>
-      </c>
-      <c r="K16" s="92"/>
+      <c r="J16" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="K16" s="85"/>
       <c r="L16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="M16" s="91" t="s">
-        <v>128</v>
-      </c>
-      <c r="N16" s="92"/>
-      <c r="O16" s="58"/>
+      <c r="M16" s="83" t="s">
+        <v>119</v>
+      </c>
+      <c r="N16" s="85"/>
+      <c r="O16" s="57"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="91" t="s">
-        <v>141</v>
-      </c>
-      <c r="D17" s="105"/>
-      <c r="E17" s="92"/>
+        <v>211</v>
+      </c>
+      <c r="C17" s="83" t="s">
+        <v>132</v>
+      </c>
+      <c r="D17" s="84"/>
+      <c r="E17" s="85"/>
       <c r="F17" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="91" t="s">
-        <v>183</v>
-      </c>
-      <c r="H17" s="92"/>
+      <c r="G17" s="83" t="s">
+        <v>166</v>
+      </c>
+      <c r="H17" s="85"/>
       <c r="I17" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="J17" s="91" t="s">
-        <v>184</v>
-      </c>
-      <c r="K17" s="92"/>
+        <v>35</v>
+      </c>
+      <c r="J17" s="83" t="s">
+        <v>167</v>
+      </c>
+      <c r="K17" s="85"/>
       <c r="L17" s="28" t="s">
-        <v>147</v>
-      </c>
-      <c r="M17" s="91" t="s">
-        <v>185</v>
-      </c>
-      <c r="N17" s="92"/>
+        <v>138</v>
+      </c>
+      <c r="M17" s="83" t="s">
+        <v>168</v>
+      </c>
+      <c r="N17" s="85"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="20" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="C18" s="93" t="s">
-        <v>180</v>
-      </c>
-      <c r="D18" s="109"/>
-      <c r="E18" s="94"/>
+        <v>102</v>
+      </c>
+      <c r="C18" s="95" t="s">
+        <v>164</v>
+      </c>
+      <c r="D18" s="96"/>
+      <c r="E18" s="97"/>
       <c r="F18" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="G18" s="93" t="s">
-        <v>146</v>
-      </c>
-      <c r="H18" s="94"/>
+      <c r="G18" s="95" t="s">
+        <v>137</v>
+      </c>
+      <c r="H18" s="97"/>
       <c r="I18" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="J18" s="93" t="s">
-        <v>181</v>
-      </c>
-      <c r="K18" s="94"/>
+        <v>133</v>
+      </c>
+      <c r="J18" s="95" t="s">
+        <v>165</v>
+      </c>
+      <c r="K18" s="97"/>
       <c r="L18" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="M18" s="93" t="s">
-        <v>186</v>
-      </c>
-      <c r="N18" s="94"/>
+        <v>204</v>
+      </c>
+      <c r="M18" s="95" t="s">
+        <v>169</v>
+      </c>
+      <c r="N18" s="97"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
-        <v>136</v>
+      <c r="A19" s="34" t="s">
+        <v>127</v>
       </c>
       <c r="B19" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="73" t="s">
-        <v>137</v>
-      </c>
-      <c r="D19" s="106"/>
-      <c r="E19" s="74"/>
+      <c r="C19" s="86" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" s="87"/>
+      <c r="E19" s="88"/>
       <c r="F19" s="26" t="s">
-        <v>112</v>
-      </c>
-      <c r="G19" s="83" t="s">
+        <v>103</v>
+      </c>
+      <c r="G19" s="102" t="s">
+        <v>131</v>
+      </c>
+      <c r="H19" s="103"/>
+      <c r="I19" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="J19" s="86" t="s">
         <v>140</v>
       </c>
-      <c r="H19" s="84"/>
-      <c r="I19" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="J19" s="73" t="s">
-        <v>150</v>
-      </c>
-      <c r="K19" s="74"/>
+      <c r="K19" s="88"/>
       <c r="L19" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="M19" s="73" t="s">
-        <v>158</v>
-      </c>
-      <c r="N19" s="74"/>
+        <v>139</v>
+      </c>
+      <c r="M19" s="86" t="s">
+        <v>146</v>
+      </c>
+      <c r="N19" s="88"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="40" t="s">
-        <v>132</v>
+      <c r="A20" s="39" t="s">
+        <v>123</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>198</v>
-      </c>
-      <c r="C20" s="85" t="s">
-        <v>138</v>
-      </c>
-      <c r="D20" s="107"/>
-      <c r="E20" s="86"/>
+        <v>178</v>
+      </c>
+      <c r="C20" s="89" t="s">
+        <v>129</v>
+      </c>
+      <c r="D20" s="90"/>
+      <c r="E20" s="91"/>
       <c r="F20" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="G20" s="85" t="s">
-        <v>144</v>
-      </c>
-      <c r="H20" s="86"/>
+        <v>108</v>
+      </c>
+      <c r="G20" s="89" t="s">
+        <v>135</v>
+      </c>
+      <c r="H20" s="91"/>
       <c r="I20" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="J20" s="79" t="s">
-        <v>151</v>
-      </c>
-      <c r="K20" s="80"/>
+        <v>108</v>
+      </c>
+      <c r="J20" s="104" t="s">
+        <v>141</v>
+      </c>
+      <c r="K20" s="105"/>
       <c r="L20" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="M20" s="75" t="s">
-        <v>159</v>
-      </c>
-      <c r="N20" s="76"/>
+        <v>108</v>
+      </c>
+      <c r="M20" s="98" t="s">
+        <v>147</v>
+      </c>
+      <c r="N20" s="99"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="39" t="s">
-        <v>133</v>
+      <c r="A21" s="38" t="s">
+        <v>124</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="C21" s="97" t="s">
-        <v>139</v>
-      </c>
-      <c r="D21" s="108"/>
-      <c r="E21" s="98"/>
+        <v>109</v>
+      </c>
+      <c r="C21" s="92" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" s="93"/>
+      <c r="E21" s="94"/>
       <c r="F21" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="G21" s="77" t="s">
-        <v>145</v>
-      </c>
-      <c r="H21" s="78"/>
+        <v>109</v>
+      </c>
+      <c r="G21" s="100" t="s">
+        <v>136</v>
+      </c>
+      <c r="H21" s="101"/>
       <c r="I21" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="J21" s="81" t="s">
-        <v>152</v>
-      </c>
-      <c r="K21" s="82"/>
+        <v>109</v>
+      </c>
+      <c r="J21" s="106" t="s">
+        <v>142</v>
+      </c>
+      <c r="K21" s="107"/>
       <c r="L21" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="M21" s="77" t="s">
-        <v>160</v>
-      </c>
-      <c r="N21" s="78"/>
+        <v>109</v>
+      </c>
+      <c r="M21" s="100" t="s">
+        <v>148</v>
+      </c>
+      <c r="N21" s="101"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="71" t="s">
-        <v>134</v>
-      </c>
-      <c r="B22" s="70" t="s">
-        <v>197</v>
-      </c>
-      <c r="C22" s="59"/>
-      <c r="D22" s="59"/>
-      <c r="E22" s="59"/>
+      <c r="A22" s="69" t="s">
+        <v>125</v>
+      </c>
+      <c r="B22" s="108" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="E22" s="58"/>
       <c r="F22" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="H22" s="50"/>
+        <v>110</v>
+      </c>
+      <c r="H22" s="49"/>
       <c r="I22" s="24" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="L22" s="24" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="B23" s="69"/>
+      <c r="A23" s="42" t="s">
+        <v>126</v>
+      </c>
+      <c r="B23" s="68"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G24" s="50"/>
-      <c r="H24" s="50"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="D25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
-      <c r="H25" s="50"/>
-      <c r="J25" s="50"/>
+      <c r="D25" s="49"/>
+      <c r="F25" s="49"/>
+      <c r="G25" s="49"/>
+      <c r="H25" s="49"/>
+      <c r="J25" s="49"/>
     </row>
     <row r="26" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="B26" s="62" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="62" t="s">
-        <v>114</v>
-      </c>
-      <c r="F26" s="62" t="s">
-        <v>65</v>
-      </c>
-      <c r="H26" s="62" t="s">
-        <v>67</v>
-      </c>
-      <c r="I26" s="62" t="s">
-        <v>73</v>
-      </c>
-      <c r="K26" s="57" t="s">
-        <v>83</v>
-      </c>
-      <c r="L26" s="57" t="s">
-        <v>93</v>
+        <v>101</v>
+      </c>
+      <c r="B26" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="61" t="s">
+        <v>105</v>
+      </c>
+      <c r="F26" s="61" t="s">
+        <v>61</v>
+      </c>
+      <c r="H26" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="I26" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="K26" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="L26" s="56" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>20</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K27" s="53" t="s">
-        <v>37</v>
-      </c>
-      <c r="L27" s="53" t="s">
-        <v>78</v>
+        <v>33</v>
+      </c>
+      <c r="K27" s="52" t="s">
+        <v>36</v>
+      </c>
+      <c r="L27" s="52" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="H28" s="7" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="I28" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="K28" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="L28" s="54" t="s">
-        <v>127</v>
+        <v>118</v>
+      </c>
+      <c r="K28" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="L28" s="53" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B29" s="22" t="s">
-        <v>50</v>
+        <v>218</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>54</v>
+        <v>216</v>
       </c>
       <c r="F29" s="22" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="H29" s="22" t="s">
-        <v>199</v>
+        <v>179</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="K29" s="55" t="s">
-        <v>39</v>
-      </c>
-      <c r="L29" s="55" t="s">
-        <v>80</v>
+        <v>67</v>
+      </c>
+      <c r="K29" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="L29" s="54" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
-        <v>49</v>
+        <v>217</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>46</v>
+        <v>220</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F30" s="23" t="s">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="H30" s="23" t="s">
         <v>22</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="K30" s="56" t="s">
-        <v>79</v>
-      </c>
-      <c r="L30" s="56" t="s">
-        <v>41</v>
+        <v>34</v>
+      </c>
+      <c r="K30" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="L30" s="55" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="87" t="s">
+      <c r="A31" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="88"/>
+      <c r="B31" s="76"/>
       <c r="C31" s="9" t="s">
         <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G31" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H31" s="87" t="s">
-        <v>66</v>
-      </c>
-      <c r="I31" s="88"/>
+      <c r="H31" s="74" t="s">
+        <v>62</v>
+      </c>
+      <c r="I31" s="76"/>
       <c r="J31" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K31" s="87" t="s">
-        <v>72</v>
-      </c>
-      <c r="L31" s="88"/>
+      <c r="K31" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="L31" s="76"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="89" t="s">
-        <v>211</v>
-      </c>
-      <c r="B32" s="90"/>
+      <c r="A32" s="77" t="s">
+        <v>191</v>
+      </c>
+      <c r="B32" s="79"/>
       <c r="C32" s="13"/>
       <c r="D32" s="3" t="s">
-        <v>214</v>
+        <v>194</v>
       </c>
       <c r="E32" s="13"/>
       <c r="F32" s="3" t="s">
-        <v>215</v>
+        <v>195</v>
       </c>
       <c r="G32" s="13"/>
-      <c r="H32" s="89" t="s">
-        <v>216</v>
-      </c>
-      <c r="I32" s="90"/>
+      <c r="H32" s="77" t="s">
+        <v>196</v>
+      </c>
+      <c r="I32" s="79"/>
       <c r="J32" s="13"/>
-      <c r="K32" s="89" t="s">
-        <v>217</v>
-      </c>
-      <c r="L32" s="90"/>
+      <c r="K32" s="77" t="s">
+        <v>197</v>
+      </c>
+      <c r="L32" s="79"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A33" s="91" t="s">
-        <v>128</v>
-      </c>
-      <c r="B33" s="92"/>
+      <c r="A33" s="83" t="s">
+        <v>119</v>
+      </c>
+      <c r="B33" s="85"/>
       <c r="C33" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="35" t="s">
-        <v>127</v>
+      <c r="D33" s="34" t="s">
+        <v>118</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F33" s="35" t="s">
-        <v>127</v>
+      <c r="F33" s="34" t="s">
+        <v>118</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="H33" s="95" t="s">
-        <v>127</v>
-      </c>
-      <c r="I33" s="96"/>
+      <c r="H33" s="80" t="s">
+        <v>118</v>
+      </c>
+      <c r="I33" s="82"/>
       <c r="J33" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K33" s="91" t="s">
-        <v>127</v>
-      </c>
-      <c r="L33" s="92"/>
+      <c r="K33" s="83" t="s">
+        <v>118</v>
+      </c>
+      <c r="L33" s="85"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A34" s="91" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="92"/>
-      <c r="C34" s="28" t="s">
-        <v>153</v>
+      <c r="A34" s="83" t="s">
+        <v>47</v>
+      </c>
+      <c r="B34" s="85"/>
+      <c r="C34" s="29" t="s">
+        <v>215</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>187</v>
+        <v>222</v>
       </c>
       <c r="E34" s="29" t="s">
-        <v>58</v>
+        <v>207</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>166</v>
-      </c>
-      <c r="G34" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="H34" s="91" t="s">
+        <v>154</v>
+      </c>
+      <c r="G34" s="29" t="s">
+        <v>229</v>
+      </c>
+      <c r="H34" s="83" t="s">
+        <v>185</v>
+      </c>
+      <c r="I34" s="85"/>
+      <c r="J34" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="K34" s="83" t="s">
+        <v>167</v>
+      </c>
+      <c r="L34" s="85"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="95" t="s">
+        <v>219</v>
+      </c>
+      <c r="B35" s="97"/>
+      <c r="C35" s="15" t="s">
         <v>205</v>
-      </c>
-      <c r="I34" s="92"/>
-      <c r="J34" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="K34" s="91" t="s">
-        <v>184</v>
-      </c>
-      <c r="L34" s="92"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A35" s="93" t="s">
-        <v>182</v>
-      </c>
-      <c r="B35" s="94"/>
-      <c r="C35" s="15" t="s">
-        <v>154</v>
       </c>
       <c r="D35" s="20" t="s">
         <v>5</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>70</v>
+        <v>208</v>
       </c>
       <c r="F35" s="20" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="G35" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="H35" s="93" t="s">
-        <v>75</v>
-      </c>
-      <c r="I35" s="94"/>
-      <c r="J35" s="33" t="s">
-        <v>113</v>
-      </c>
-      <c r="K35" s="93" t="s">
-        <v>188</v>
-      </c>
-      <c r="L35" s="94"/>
+        <v>150</v>
+      </c>
+      <c r="H35" s="95" t="s">
+        <v>68</v>
+      </c>
+      <c r="I35" s="97"/>
+      <c r="J35" s="32" t="s">
+        <v>104</v>
+      </c>
+      <c r="K35" s="95" t="s">
+        <v>170</v>
+      </c>
+      <c r="L35" s="97"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A36" s="73" t="s">
+      <c r="A36" s="86" t="s">
+        <v>224</v>
+      </c>
+      <c r="B36" s="88"/>
+      <c r="C36" s="27" t="s">
+        <v>143</v>
+      </c>
+      <c r="D36" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="E36" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="F36" s="43" t="s">
+        <v>182</v>
+      </c>
+      <c r="G36" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="H36" s="89" t="s">
+        <v>153</v>
+      </c>
+      <c r="I36" s="91"/>
+      <c r="J36" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="K36" s="86" t="s">
         <v>158</v>
       </c>
-      <c r="B36" s="74"/>
-      <c r="C36" s="27" t="s">
+      <c r="L36" s="88"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="98" t="s">
+        <v>221</v>
+      </c>
+      <c r="B37" s="99"/>
+      <c r="C37" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" s="66" t="s">
+        <v>174</v>
+      </c>
+      <c r="E37" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="F37" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="G37" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="H37" s="89" t="s">
         <v>155</v>
       </c>
-      <c r="D36" s="68" t="s">
-        <v>55</v>
-      </c>
-      <c r="E36" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="F36" s="44" t="s">
-        <v>202</v>
-      </c>
-      <c r="G36" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="H36" s="85" t="s">
-        <v>165</v>
-      </c>
-      <c r="I36" s="86"/>
-      <c r="J36" s="45" t="s">
-        <v>168</v>
-      </c>
-      <c r="K36" s="73" t="s">
-        <v>170</v>
-      </c>
-      <c r="L36" s="74"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A37" s="75" t="s">
+      <c r="I37" s="91"/>
+      <c r="J37" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="K37" s="89" t="s">
         <v>159</v>
       </c>
-      <c r="B37" s="76"/>
-      <c r="C37" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="D37" s="67" t="s">
-        <v>194</v>
-      </c>
-      <c r="E37" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="F37" s="40" t="s">
-        <v>203</v>
-      </c>
-      <c r="G37" s="33" t="s">
-        <v>69</v>
-      </c>
-      <c r="H37" s="85" t="s">
-        <v>167</v>
-      </c>
-      <c r="I37" s="86"/>
-      <c r="J37" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="K37" s="85" t="s">
-        <v>171</v>
-      </c>
-      <c r="L37" s="86"/>
+      <c r="L37" s="91"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A38" s="77" t="s">
+      <c r="A38" s="100" t="s">
+        <v>223</v>
+      </c>
+      <c r="B38" s="101"/>
+      <c r="C38" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="63" t="s">
+        <v>118</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="F38" s="42" t="s">
+        <v>184</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="H38" s="92" t="s">
+        <v>157</v>
+      </c>
+      <c r="I38" s="94"/>
+      <c r="J38" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="K38" s="92" t="s">
         <v>160</v>
       </c>
-      <c r="B38" s="78"/>
-      <c r="C38" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="D38" s="64" t="s">
-        <v>127</v>
-      </c>
-      <c r="E38" s="30" t="s">
-        <v>63</v>
-      </c>
-      <c r="F38" s="43" t="s">
-        <v>204</v>
-      </c>
-      <c r="G38" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="H38" s="97" t="s">
-        <v>169</v>
-      </c>
-      <c r="I38" s="98"/>
-      <c r="J38" s="25" t="s">
-        <v>118</v>
-      </c>
-      <c r="K38" s="97" t="s">
-        <v>173</v>
-      </c>
-      <c r="L38" s="98"/>
+      <c r="L38" s="94"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C39" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="D39" s="65" t="s">
-        <v>56</v>
+        <v>110</v>
+      </c>
+      <c r="D39" s="64" t="s">
+        <v>54</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="F39" s="50"/>
+        <v>214</v>
+      </c>
+      <c r="F39" s="49"/>
       <c r="G39" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="H39" s="50"/>
+        <v>110</v>
+      </c>
+      <c r="H39" s="49"/>
       <c r="J39" s="24" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D40" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="F40" s="50"/>
-      <c r="H40" s="50"/>
+      <c r="D40" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="F40" s="49"/>
+      <c r="H40" s="49"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D41" s="50"/>
-      <c r="J41" s="50"/>
+      <c r="D41" s="49"/>
+      <c r="J41" s="49"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D42" s="50"/>
+      <c r="D42" s="49"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D43" s="50"/>
-      <c r="F43" s="50"/>
-      <c r="H43" s="50"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="50"/>
+      <c r="D43" s="49"/>
+      <c r="F43" s="49"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
     </row>
     <row r="44" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A44" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B44" s="62" t="s">
-        <v>93</v>
-      </c>
-      <c r="D44" s="62" t="s">
-        <v>94</v>
-      </c>
-      <c r="E44" s="62" t="s">
-        <v>122</v>
-      </c>
-      <c r="G44" s="62" t="s">
-        <v>95</v>
-      </c>
-      <c r="I44" s="62" t="s">
-        <v>97</v>
-      </c>
-      <c r="K44" s="62" t="s">
-        <v>123</v>
+        <v>75</v>
+      </c>
+      <c r="B44" s="61" t="s">
+        <v>84</v>
+      </c>
+      <c r="D44" s="61" t="s">
+        <v>85</v>
+      </c>
+      <c r="E44" s="61" t="s">
+        <v>113</v>
+      </c>
+      <c r="G44" s="61" t="s">
+        <v>86</v>
+      </c>
+      <c r="I44" s="61" t="s">
+        <v>88</v>
+      </c>
+      <c r="K44" s="61" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>28</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K45" s="6" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="D46" s="7" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="E46" s="7" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="G46" s="7" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="I46" s="7" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="K46" s="7" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="22" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D47" s="22" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E47" s="22" t="s">
-        <v>209</v>
+        <v>189</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>61</v>
+        <v>212</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="K47" s="22" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="23" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="G48" s="23" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="K48" s="23" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="87" t="s">
-        <v>72</v>
-      </c>
-      <c r="B49" s="88"/>
+      <c r="A49" s="74" t="s">
+        <v>65</v>
+      </c>
+      <c r="B49" s="76"/>
       <c r="C49" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D49" s="87" t="s">
+      <c r="D49" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="E49" s="88"/>
+      <c r="E49" s="76"/>
       <c r="F49" s="9" t="s">
         <v>10</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H49" s="9" t="s">
         <v>10</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J49" s="9" t="s">
         <v>10</v>
       </c>
       <c r="K49" s="1" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="89" t="s">
-        <v>218</v>
-      </c>
-      <c r="B50" s="90"/>
+      <c r="A50" s="77" t="s">
+        <v>198</v>
+      </c>
+      <c r="B50" s="79"/>
       <c r="C50" s="13"/>
-      <c r="D50" s="89" t="s">
-        <v>219</v>
-      </c>
-      <c r="E50" s="90"/>
+      <c r="D50" s="77" t="s">
+        <v>199</v>
+      </c>
+      <c r="E50" s="79"/>
       <c r="F50" s="13"/>
       <c r="G50" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H50" s="13"/>
       <c r="I50" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J50" s="13"/>
       <c r="K50" s="3" t="s">
-        <v>220</v>
+        <v>200</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="91" t="s">
-        <v>127</v>
-      </c>
-      <c r="B51" s="92"/>
+      <c r="A51" s="83" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51" s="85"/>
       <c r="C51" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D51" s="91" t="s">
-        <v>129</v>
-      </c>
-      <c r="E51" s="92"/>
+      <c r="D51" s="83" t="s">
+        <v>120</v>
+      </c>
+      <c r="E51" s="85"/>
       <c r="F51" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G51" s="35" t="s">
-        <v>130</v>
+      <c r="G51" s="34" t="s">
+        <v>121</v>
       </c>
       <c r="H51" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I51" s="35" t="s">
-        <v>130</v>
+      <c r="I51" s="34" t="s">
+        <v>121</v>
       </c>
       <c r="J51" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="K51" s="35" t="s">
+      <c r="K51" s="34" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="91" t="s">
-        <v>77</v>
-      </c>
-      <c r="B52" s="92"/>
+      <c r="A52" s="83" t="s">
+        <v>69</v>
+      </c>
+      <c r="B52" s="85"/>
       <c r="C52" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="D52" s="91" t="s">
-        <v>189</v>
-      </c>
-      <c r="E52" s="92"/>
+        <v>73</v>
+      </c>
+      <c r="D52" s="83" t="s">
+        <v>171</v>
+      </c>
+      <c r="E52" s="85"/>
       <c r="F52" s="28" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="G52" s="21" t="s">
-        <v>90</v>
+        <v>213</v>
       </c>
       <c r="H52" s="29" t="s">
-        <v>58</v>
+        <v>207</v>
       </c>
       <c r="I52" s="21" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="J52" s="11" t="s">
-        <v>192</v>
+        <v>228</v>
       </c>
       <c r="K52" s="21" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" s="91" t="s">
-        <v>188</v>
-      </c>
-      <c r="B53" s="92"/>
+      <c r="A53" s="83" t="s">
+        <v>170</v>
+      </c>
+      <c r="B53" s="85"/>
       <c r="C53" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D53" s="95" t="s">
+        <v>210</v>
+      </c>
+      <c r="E53" s="97"/>
+      <c r="F53" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="G53" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="D53" s="93" t="s">
-        <v>190</v>
-      </c>
-      <c r="E53" s="94"/>
-      <c r="F53" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="G53" s="20" t="s">
+      <c r="H53" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="I53" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="H53" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="I53" s="20" t="s">
-        <v>100</v>
-      </c>
       <c r="J53" s="15" t="s">
-        <v>191</v>
+        <v>172</v>
       </c>
       <c r="K53" s="20" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="73" t="s">
-        <v>170</v>
-      </c>
-      <c r="B54" s="74"/>
+      <c r="A54" s="86" t="s">
+        <v>158</v>
+      </c>
+      <c r="B54" s="88"/>
       <c r="C54" s="26" t="s">
-        <v>172</v>
-      </c>
-      <c r="D54" s="73" t="s">
-        <v>176</v>
-      </c>
-      <c r="E54" s="74"/>
+        <v>206</v>
+      </c>
+      <c r="D54" s="86" t="s">
+        <v>225</v>
+      </c>
+      <c r="E54" s="88"/>
       <c r="F54" s="27" t="s">
-        <v>87</v>
-      </c>
-      <c r="G54" s="68" t="s">
-        <v>55</v>
+        <v>79</v>
+      </c>
+      <c r="G54" s="67" t="s">
+        <v>53</v>
       </c>
       <c r="H54" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="I54" s="39" t="s">
-        <v>222</v>
+        <v>209</v>
+      </c>
+      <c r="I54" s="38" t="s">
+        <v>202</v>
       </c>
       <c r="J54" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K54" s="99" t="s">
-        <v>106</v>
+      <c r="K54" s="71" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="85" t="s">
-        <v>171</v>
-      </c>
-      <c r="B55" s="86"/>
+      <c r="A55" s="89" t="s">
+        <v>159</v>
+      </c>
+      <c r="B55" s="91"/>
       <c r="C55" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="D55" s="75" t="s">
-        <v>177</v>
-      </c>
-      <c r="E55" s="76"/>
+        <v>108</v>
+      </c>
+      <c r="D55" s="98" t="s">
+        <v>226</v>
+      </c>
+      <c r="E55" s="99"/>
       <c r="F55" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="G55" s="63" t="s">
-        <v>195</v>
+        <v>108</v>
+      </c>
+      <c r="G55" s="62" t="s">
+        <v>175</v>
       </c>
       <c r="H55" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="I55" s="39" t="s">
-        <v>223</v>
+        <v>108</v>
+      </c>
+      <c r="I55" s="38" t="s">
+        <v>203</v>
       </c>
       <c r="J55" s="25" t="s">
-        <v>117</v>
-      </c>
-      <c r="K55" s="100"/>
+        <v>108</v>
+      </c>
+      <c r="K55" s="72"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" s="97" t="s">
-        <v>173</v>
-      </c>
-      <c r="B56" s="98"/>
+      <c r="A56" s="92" t="s">
+        <v>160</v>
+      </c>
+      <c r="B56" s="94"/>
       <c r="C56" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="D56" s="77" t="s">
-        <v>178</v>
-      </c>
-      <c r="E56" s="78"/>
+        <v>109</v>
+      </c>
+      <c r="D56" s="100" t="s">
+        <v>227</v>
+      </c>
+      <c r="E56" s="101"/>
       <c r="F56" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="G56" s="64" t="s">
-        <v>130</v>
+        <v>109</v>
+      </c>
+      <c r="G56" s="63" t="s">
+        <v>121</v>
       </c>
       <c r="H56" s="30" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J56" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="K56" s="61" t="s">
-        <v>107</v>
+        <v>109</v>
+      </c>
+      <c r="K56" s="60" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C57" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="D57" s="50"/>
+        <v>110</v>
+      </c>
+      <c r="D57" s="49"/>
       <c r="F57" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="G57" s="65" t="s">
-        <v>88</v>
+        <v>110</v>
+      </c>
+      <c r="G57" s="64" t="s">
+        <v>80</v>
       </c>
       <c r="H57" s="24" t="s">
-        <v>64</v>
+        <v>214</v>
       </c>
       <c r="J57" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="K57" s="50"/>
+        <v>110</v>
+      </c>
+      <c r="K57" s="49"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D58" s="50"/>
-      <c r="G58" s="66" t="s">
-        <v>89</v>
-      </c>
-      <c r="H58" s="50"/>
-      <c r="I58" s="50"/>
-      <c r="J58" s="50"/>
+      <c r="D58" s="49"/>
+      <c r="G58" s="65" t="s">
+        <v>81</v>
+      </c>
+      <c r="H58" s="49"/>
+      <c r="I58" s="49"/>
+      <c r="J58" s="49"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="F59" s="50"/>
+      <c r="F59" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="74">
+    <mergeCell ref="M19:N19"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J20:K20"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="J18:K18"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A54:B54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="K36:L36"/>
+    <mergeCell ref="K37:L37"/>
+    <mergeCell ref="K38:L38"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="H36:I36"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="K31:L31"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="K33:L33"/>
+    <mergeCell ref="K34:L34"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="H31:I31"/>
+    <mergeCell ref="H32:I32"/>
+    <mergeCell ref="H33:I33"/>
+    <mergeCell ref="H34:I34"/>
+    <mergeCell ref="H35:I35"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="M18:N18"/>
     <mergeCell ref="K54:K55"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="C14:E14"/>
@@ -4125,72 +4394,14 @@
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A36:B36"/>
-    <mergeCell ref="M14:N14"/>
-    <mergeCell ref="M15:N15"/>
-    <mergeCell ref="M16:N16"/>
-    <mergeCell ref="M17:N17"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="H31:I31"/>
-    <mergeCell ref="H32:I32"/>
-    <mergeCell ref="H33:I33"/>
-    <mergeCell ref="H34:I34"/>
-    <mergeCell ref="H35:I35"/>
-    <mergeCell ref="K31:L31"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="K33:L33"/>
-    <mergeCell ref="K34:L34"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K36:L36"/>
-    <mergeCell ref="K37:L37"/>
-    <mergeCell ref="K38:L38"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="H36:I36"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="J18:K18"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="M19:N19"/>
-    <mergeCell ref="M20:N20"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="J19:K19"/>
-    <mergeCell ref="J20:K20"/>
-    <mergeCell ref="J21:K21"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{22769755-18A0-4228-9384-568445F69ECC}"/>
-    <hyperlink ref="B5" r:id="rId2" xr:uid="{03E9F580-BDD7-4231-87F7-C1F4E6AE31D0}"/>
-    <hyperlink ref="B6" r:id="rId3" xr:uid="{77F85450-50CF-45C9-8D04-92B93616F32E}"/>
-    <hyperlink ref="B7" r:id="rId4" xr:uid="{C8FB0067-ED59-4BC0-8C56-F67274EB48A8}"/>
-    <hyperlink ref="B4" r:id="rId5" xr:uid="{DFEC60C0-6336-4B8F-A83F-DC250E52EDE6}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{EC28AFA3-8E64-4B66-A9DA-F5A51E377CE6}"/>
+    <hyperlink ref="B3" r:id="rId1"/>
+    <hyperlink ref="B5" r:id="rId2"/>
+    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B7" r:id="rId4"/>
+    <hyperlink ref="B4" r:id="rId5"/>
+    <hyperlink ref="C6" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId7"/>

</xml_diff>